<commit_message>
Added Max usage feature
</commit_message>
<xml_diff>
--- a/BrickMapMaker/BrickList.xlsx
+++ b/BrickMapMaker/BrickList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\Dropbox\DevProjects\BrickMapMaker\BrickMapMaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C842C9ED-A339-4928-8872-DD59EBF97567}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE9CF70-53A4-4A1B-81A5-115792E2FFB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6435" yWindow="2550" windowWidth="18435" windowHeight="12810" activeTab="1" xr2:uid="{AC5AA4F4-2ADF-460C-8C37-B528CCEA2721}"/>
+    <workbookView xWindow="6435" yWindow="2550" windowWidth="18435" windowHeight="12810" xr2:uid="{AC5AA4F4-2ADF-460C-8C37-B528CCEA2721}"/>
   </bookViews>
   <sheets>
     <sheet name="ElementData" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="97">
   <si>
     <t>DesignId</t>
   </si>
@@ -318,6 +318,12 @@
   </si>
   <si>
     <t>0,0,1,0,1,0,-1,0,0,{0},-0.64,{1}</t>
+  </si>
+  <si>
+    <t>12 kr st på BL</t>
+  </si>
+  <si>
+    <t>8 kr st på BL</t>
   </si>
 </sst>
 </file>
@@ -689,11 +695,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FBD227-4711-4E5E-9A37-426C729051A6}">
-  <dimension ref="A1:J313"/>
+  <dimension ref="A1:J314"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,6 +708,7 @@
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1695,13 +1702,13 @@
         <v>28</v>
       </c>
       <c r="B59">
-        <v>3024</v>
+        <v>2445</v>
       </c>
       <c r="C59">
-        <v>3000</v>
+        <v>4</v>
       </c>
       <c r="D59">
-        <v>302428</v>
+        <v>6218146</v>
       </c>
       <c r="E59" t="s">
         <v>42</v>
@@ -1712,13 +1719,13 @@
         <v>28</v>
       </c>
       <c r="B60">
-        <v>3023</v>
+        <v>3020</v>
       </c>
       <c r="C60">
         <v>3000</v>
       </c>
       <c r="D60">
-        <v>302328</v>
+        <v>302028</v>
       </c>
       <c r="E60" t="s">
         <v>42</v>
@@ -1729,13 +1736,13 @@
         <v>28</v>
       </c>
       <c r="B61">
-        <v>3623</v>
+        <v>3021</v>
       </c>
       <c r="C61">
         <v>3000</v>
       </c>
       <c r="D61">
-        <v>4107758</v>
+        <v>302128</v>
       </c>
       <c r="E61" t="s">
         <v>42</v>
@@ -1746,13 +1753,13 @@
         <v>28</v>
       </c>
       <c r="B62">
-        <v>3710</v>
+        <v>3022</v>
       </c>
       <c r="C62">
         <v>3000</v>
       </c>
       <c r="D62">
-        <v>371028</v>
+        <v>302228</v>
       </c>
       <c r="E62" t="s">
         <v>42</v>
@@ -1763,13 +1770,13 @@
         <v>28</v>
       </c>
       <c r="B63">
-        <v>3666</v>
+        <v>3023</v>
       </c>
       <c r="C63">
         <v>3000</v>
       </c>
       <c r="D63">
-        <v>366628</v>
+        <v>302328</v>
       </c>
       <c r="E63" t="s">
         <v>42</v>
@@ -1780,13 +1787,13 @@
         <v>28</v>
       </c>
       <c r="B64">
-        <v>3460</v>
+        <v>3024</v>
       </c>
       <c r="C64">
         <v>3000</v>
       </c>
       <c r="D64">
-        <v>346028</v>
+        <v>302428</v>
       </c>
       <c r="E64" t="s">
         <v>42</v>
@@ -1797,13 +1804,13 @@
         <v>28</v>
       </c>
       <c r="B65">
-        <v>3022</v>
+        <v>3027</v>
       </c>
       <c r="C65">
-        <v>3000</v>
+        <v>1</v>
       </c>
       <c r="D65">
-        <v>302228</v>
+        <v>0</v>
       </c>
       <c r="E65" t="s">
         <v>42</v>
@@ -1814,16 +1821,19 @@
         <v>28</v>
       </c>
       <c r="B66">
-        <v>3021</v>
+        <v>3028</v>
       </c>
       <c r="C66">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="D66">
-        <v>302128</v>
+        <v>6177783</v>
       </c>
       <c r="E66" t="s">
         <v>42</v>
+      </c>
+      <c r="F66" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -1831,13 +1841,13 @@
         <v>28</v>
       </c>
       <c r="B67">
-        <v>3020</v>
+        <v>3029</v>
       </c>
       <c r="C67">
-        <v>3000</v>
+        <v>9</v>
       </c>
       <c r="D67">
-        <v>302028</v>
+        <v>4279059</v>
       </c>
       <c r="E67" t="s">
         <v>42</v>
@@ -1848,16 +1858,19 @@
         <v>28</v>
       </c>
       <c r="B68">
-        <v>3795</v>
+        <v>3030</v>
       </c>
       <c r="C68">
-        <v>3000</v>
+        <v>7</v>
       </c>
       <c r="D68">
-        <v>379528</v>
+        <v>6247196</v>
       </c>
       <c r="E68" t="s">
         <v>42</v>
+      </c>
+      <c r="F68" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -1865,13 +1878,13 @@
         <v>28</v>
       </c>
       <c r="B69">
-        <v>3034</v>
+        <v>3031</v>
       </c>
       <c r="C69">
-        <v>3000</v>
+        <v>75</v>
       </c>
       <c r="D69">
-        <v>303428</v>
+        <v>4243821</v>
       </c>
       <c r="E69" t="s">
         <v>42</v>
@@ -1882,13 +1895,13 @@
         <v>28</v>
       </c>
       <c r="B70">
-        <v>3832</v>
+        <v>3032</v>
       </c>
       <c r="C70">
-        <v>3000</v>
+        <v>36</v>
       </c>
       <c r="D70">
-        <v>383228</v>
+        <v>4116671</v>
       </c>
       <c r="E70" t="s">
         <v>42</v>
@@ -1899,13 +1912,13 @@
         <v>28</v>
       </c>
       <c r="B71">
-        <v>2445</v>
+        <v>3034</v>
       </c>
       <c r="C71">
-        <v>3000</v>
+        <v>45</v>
       </c>
       <c r="D71">
-        <v>6218146</v>
+        <v>303428</v>
       </c>
       <c r="E71" t="s">
         <v>42</v>
@@ -1916,49 +1929,48 @@
         <v>28</v>
       </c>
       <c r="B72">
-        <v>3031</v>
+        <v>3035</v>
       </c>
       <c r="C72">
-        <v>3000</v>
+        <v>16</v>
       </c>
       <c r="D72">
-        <v>4243821</v>
+        <v>4277361</v>
       </c>
       <c r="E72" t="s">
         <v>42</v>
       </c>
-      <c r="I72" s="1"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>28</v>
       </c>
       <c r="B73">
-        <v>3032</v>
+        <v>3036</v>
       </c>
       <c r="C73">
-        <v>3000</v>
+        <v>17</v>
       </c>
       <c r="D73">
-        <v>4116671</v>
+        <v>4507311</v>
       </c>
       <c r="E73" t="s">
         <v>42</v>
       </c>
-      <c r="J73" s="1"/>
+      <c r="I73" s="1"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>28</v>
       </c>
       <c r="B74">
-        <v>3035</v>
+        <v>3460</v>
       </c>
       <c r="C74">
-        <v>3000</v>
+        <v>4</v>
       </c>
       <c r="D74">
-        <v>4277361</v>
+        <v>346028</v>
       </c>
       <c r="E74" t="s">
         <v>42</v>
@@ -1970,30 +1982,31 @@
         <v>28</v>
       </c>
       <c r="B75">
-        <v>3030</v>
+        <v>3623</v>
       </c>
       <c r="C75">
         <v>3000</v>
       </c>
       <c r="D75">
-        <v>6247196</v>
+        <v>4107758</v>
       </c>
       <c r="E75" t="s">
         <v>42</v>
       </c>
+      <c r="J75" s="1"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>28</v>
       </c>
       <c r="B76">
-        <v>3029</v>
+        <v>3666</v>
       </c>
       <c r="C76">
         <v>3000</v>
       </c>
       <c r="D76">
-        <v>4279059</v>
+        <v>366628</v>
       </c>
       <c r="E76" t="s">
         <v>42</v>
@@ -2004,13 +2017,13 @@
         <v>28</v>
       </c>
       <c r="B77">
-        <v>3958</v>
+        <v>3710</v>
       </c>
       <c r="C77">
         <v>3000</v>
       </c>
       <c r="D77">
-        <v>6097194</v>
+        <v>371028</v>
       </c>
       <c r="E77" t="s">
         <v>42</v>
@@ -2021,13 +2034,13 @@
         <v>28</v>
       </c>
       <c r="B78">
-        <v>3036</v>
+        <v>3795</v>
       </c>
       <c r="C78">
-        <v>3000</v>
+        <v>127</v>
       </c>
       <c r="D78">
-        <v>4507311</v>
+        <v>379528</v>
       </c>
       <c r="E78" t="s">
         <v>42</v>
@@ -2038,13 +2051,13 @@
         <v>28</v>
       </c>
       <c r="B79">
-        <v>3028</v>
+        <v>3832</v>
       </c>
       <c r="C79">
-        <v>3000</v>
+        <v>16</v>
       </c>
       <c r="D79">
-        <v>6177783</v>
+        <v>383228</v>
       </c>
       <c r="E79" t="s">
         <v>42</v>
@@ -2055,13 +2068,13 @@
         <v>28</v>
       </c>
       <c r="B80">
-        <v>41539</v>
+        <v>3958</v>
       </c>
       <c r="C80">
-        <v>3000</v>
+        <v>14</v>
       </c>
       <c r="D80">
-        <v>4161677</v>
+        <v>6097194</v>
       </c>
       <c r="E80" t="s">
         <v>42</v>
@@ -2072,13 +2085,13 @@
         <v>28</v>
       </c>
       <c r="B81">
-        <v>92438</v>
+        <v>41539</v>
       </c>
       <c r="C81">
-        <v>3000</v>
+        <v>20</v>
       </c>
       <c r="D81">
-        <v>4610602</v>
+        <v>4161677</v>
       </c>
       <c r="E81" t="s">
         <v>42</v>
@@ -2092,7 +2105,7 @@
         <v>91405</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D82" s="2">
         <v>4626702</v>
@@ -2103,69 +2116,69 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B83">
-        <v>3024</v>
+        <v>92438</v>
       </c>
       <c r="C83">
-        <v>0</v>
-      </c>
-      <c r="D83" s="1">
-        <v>6223741</v>
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <v>4610602</v>
       </c>
       <c r="E83" t="s">
-        <v>44</v>
-      </c>
-      <c r="I83" s="1"/>
+        <v>42</v>
+      </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>37</v>
       </c>
       <c r="B84">
-        <v>3710</v>
+        <v>3024</v>
       </c>
       <c r="C84">
         <v>0</v>
       </c>
       <c r="D84" s="1">
-        <v>6138515</v>
+        <v>6223741</v>
       </c>
       <c r="E84" t="s">
         <v>44</v>
       </c>
-      <c r="F84" s="1"/>
+      <c r="I84" s="1"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>37</v>
       </c>
       <c r="B85">
-        <v>3020</v>
+        <v>3710</v>
       </c>
       <c r="C85">
-        <v>3000</v>
-      </c>
-      <c r="D85">
-        <v>6141590</v>
+        <v>0</v>
+      </c>
+      <c r="D85" s="1">
+        <v>6138515</v>
       </c>
       <c r="E85" t="s">
         <v>44</v>
       </c>
+      <c r="F85" s="1"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>37</v>
       </c>
       <c r="B86">
-        <v>3031</v>
+        <v>3020</v>
       </c>
       <c r="C86">
         <v>3000</v>
       </c>
       <c r="D86">
-        <v>4617799</v>
+        <v>6141590</v>
       </c>
       <c r="E86" t="s">
         <v>44</v>
@@ -2176,86 +2189,86 @@
         <v>37</v>
       </c>
       <c r="B87">
-        <v>3958</v>
+        <v>3031</v>
       </c>
       <c r="C87">
         <v>3000</v>
       </c>
       <c r="D87">
-        <v>6004650</v>
+        <v>4617799</v>
       </c>
       <c r="E87" t="s">
         <v>44</v>
       </c>
-      <c r="F87" s="1"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>37</v>
       </c>
       <c r="B88">
-        <v>3028</v>
+        <v>3958</v>
       </c>
       <c r="C88">
         <v>3000</v>
       </c>
       <c r="D88">
-        <v>4541414</v>
+        <v>6004650</v>
       </c>
       <c r="E88" t="s">
         <v>44</v>
       </c>
+      <c r="F88" s="1"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>37</v>
       </c>
       <c r="B89">
-        <v>92438</v>
+        <v>3028</v>
       </c>
       <c r="C89">
         <v>3000</v>
       </c>
       <c r="D89">
-        <v>4610353</v>
+        <v>4541414</v>
       </c>
       <c r="E89" t="s">
         <v>44</v>
       </c>
-      <c r="I89" s="1"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>37</v>
       </c>
       <c r="B90">
-        <v>91405</v>
+        <v>92438</v>
       </c>
       <c r="C90">
         <v>3000</v>
       </c>
       <c r="D90">
-        <v>4611777</v>
+        <v>4610353</v>
       </c>
       <c r="E90" t="s">
         <v>44</v>
       </c>
+      <c r="I90" s="1"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>138</v>
+        <v>37</v>
       </c>
       <c r="B91">
-        <v>3024</v>
+        <v>91405</v>
       </c>
       <c r="C91">
         <v>3000</v>
       </c>
       <c r="D91">
-        <v>4549436</v>
+        <v>4611777</v>
       </c>
       <c r="E91" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -2263,13 +2276,13 @@
         <v>138</v>
       </c>
       <c r="B92">
-        <v>3023</v>
+        <v>3024</v>
       </c>
       <c r="C92">
         <v>3000</v>
       </c>
       <c r="D92">
-        <v>4528604</v>
+        <v>4549436</v>
       </c>
       <c r="E92" t="s">
         <v>45</v>
@@ -2280,13 +2293,13 @@
         <v>138</v>
       </c>
       <c r="B93">
-        <v>3623</v>
+        <v>3023</v>
       </c>
       <c r="C93">
         <v>3000</v>
       </c>
       <c r="D93">
-        <v>6132768</v>
+        <v>4528604</v>
       </c>
       <c r="E93" t="s">
         <v>45</v>
@@ -2297,13 +2310,13 @@
         <v>138</v>
       </c>
       <c r="B94">
-        <v>3710</v>
+        <v>3623</v>
       </c>
       <c r="C94">
         <v>3000</v>
       </c>
       <c r="D94">
-        <v>4626904</v>
+        <v>6132768</v>
       </c>
       <c r="E94" t="s">
         <v>45</v>
@@ -2314,13 +2327,13 @@
         <v>138</v>
       </c>
       <c r="B95">
-        <v>3666</v>
+        <v>3710</v>
       </c>
       <c r="C95">
         <v>3000</v>
       </c>
       <c r="D95">
-        <v>6015424</v>
+        <v>4626904</v>
       </c>
       <c r="E95" t="s">
         <v>45</v>
@@ -2331,13 +2344,13 @@
         <v>138</v>
       </c>
       <c r="B96">
-        <v>3460</v>
+        <v>3666</v>
       </c>
       <c r="C96">
         <v>3000</v>
       </c>
       <c r="D96">
-        <v>6156492</v>
+        <v>6015424</v>
       </c>
       <c r="E96" t="s">
         <v>45</v>
@@ -2348,13 +2361,13 @@
         <v>138</v>
       </c>
       <c r="B97">
-        <v>60479</v>
+        <v>3460</v>
       </c>
       <c r="C97">
         <v>3000</v>
       </c>
       <c r="D97">
-        <v>6275088</v>
+        <v>6156492</v>
       </c>
       <c r="E97" t="s">
         <v>45</v>
@@ -2365,13 +2378,13 @@
         <v>138</v>
       </c>
       <c r="B98">
-        <v>3022</v>
+        <v>60479</v>
       </c>
       <c r="C98">
         <v>3000</v>
       </c>
       <c r="D98">
-        <v>6047415</v>
+        <v>6275088</v>
       </c>
       <c r="E98" t="s">
         <v>45</v>
@@ -2382,13 +2395,13 @@
         <v>138</v>
       </c>
       <c r="B99">
-        <v>3021</v>
+        <v>3022</v>
       </c>
       <c r="C99">
         <v>3000</v>
       </c>
       <c r="D99">
-        <v>6035540</v>
+        <v>6047415</v>
       </c>
       <c r="E99" t="s">
         <v>45</v>
@@ -2399,13 +2412,13 @@
         <v>138</v>
       </c>
       <c r="B100">
-        <v>3020</v>
+        <v>3021</v>
       </c>
       <c r="C100">
         <v>3000</v>
       </c>
       <c r="D100">
-        <v>4267874</v>
+        <v>6035540</v>
       </c>
       <c r="E100" t="s">
         <v>45</v>
@@ -2416,13 +2429,13 @@
         <v>138</v>
       </c>
       <c r="B101">
-        <v>3795</v>
+        <v>3020</v>
       </c>
       <c r="C101">
         <v>3000</v>
       </c>
       <c r="D101">
-        <v>4550329</v>
+        <v>4267874</v>
       </c>
       <c r="E101" t="s">
         <v>45</v>
@@ -2433,13 +2446,13 @@
         <v>138</v>
       </c>
       <c r="B102">
-        <v>3034</v>
+        <v>3795</v>
       </c>
       <c r="C102">
         <v>3000</v>
       </c>
       <c r="D102">
-        <v>4246957</v>
+        <v>4550329</v>
       </c>
       <c r="E102" t="s">
         <v>45</v>
@@ -2450,13 +2463,13 @@
         <v>138</v>
       </c>
       <c r="B103">
-        <v>3832</v>
+        <v>3034</v>
       </c>
       <c r="C103">
-        <v>0</v>
-      </c>
-      <c r="D103" s="1">
-        <v>6079776</v>
+        <v>3000</v>
+      </c>
+      <c r="D103">
+        <v>4246957</v>
       </c>
       <c r="E103" t="s">
         <v>45</v>
@@ -2467,13 +2480,13 @@
         <v>138</v>
       </c>
       <c r="B104">
-        <v>2445</v>
+        <v>3832</v>
       </c>
       <c r="C104">
         <v>0</v>
       </c>
       <c r="D104" s="1">
-        <v>4268715</v>
+        <v>6079776</v>
       </c>
       <c r="E104" t="s">
         <v>45</v>
@@ -2484,13 +2497,13 @@
         <v>138</v>
       </c>
       <c r="B105">
-        <v>3032</v>
+        <v>2445</v>
       </c>
       <c r="C105">
-        <v>3000</v>
-      </c>
-      <c r="D105">
-        <v>6167894</v>
+        <v>0</v>
+      </c>
+      <c r="D105" s="1">
+        <v>4268715</v>
       </c>
       <c r="E105" t="s">
         <v>45</v>
@@ -2501,13 +2514,13 @@
         <v>138</v>
       </c>
       <c r="B106">
-        <v>3030</v>
+        <v>3032</v>
       </c>
       <c r="C106">
         <v>3000</v>
       </c>
       <c r="D106">
-        <v>6001001</v>
+        <v>6167894</v>
       </c>
       <c r="E106" t="s">
         <v>45</v>
@@ -2518,13 +2531,13 @@
         <v>138</v>
       </c>
       <c r="B107">
-        <v>3029</v>
+        <v>3030</v>
       </c>
       <c r="C107">
         <v>3000</v>
       </c>
       <c r="D107">
-        <v>6114515</v>
+        <v>6001001</v>
       </c>
       <c r="E107" t="s">
         <v>45</v>
@@ -2535,13 +2548,13 @@
         <v>138</v>
       </c>
       <c r="B108">
-        <v>3958</v>
+        <v>3029</v>
       </c>
       <c r="C108">
         <v>3000</v>
       </c>
       <c r="D108">
-        <v>4530712</v>
+        <v>6114515</v>
       </c>
       <c r="E108" t="s">
         <v>45</v>
@@ -2552,13 +2565,13 @@
         <v>138</v>
       </c>
       <c r="B109">
-        <v>3036</v>
+        <v>3958</v>
       </c>
       <c r="C109">
         <v>3000</v>
       </c>
       <c r="D109">
-        <v>4251796</v>
+        <v>4530712</v>
       </c>
       <c r="E109" t="s">
         <v>45</v>
@@ -2569,13 +2582,13 @@
         <v>138</v>
       </c>
       <c r="B110">
-        <v>3033</v>
+        <v>3036</v>
       </c>
       <c r="C110">
         <v>3000</v>
       </c>
       <c r="D110">
-        <v>6096215</v>
+        <v>4251796</v>
       </c>
       <c r="E110" t="s">
         <v>45</v>
@@ -2586,13 +2599,13 @@
         <v>138</v>
       </c>
       <c r="B111">
-        <v>41539</v>
+        <v>3033</v>
       </c>
       <c r="C111">
         <v>3000</v>
       </c>
       <c r="D111">
-        <v>4570111</v>
+        <v>6096215</v>
       </c>
       <c r="E111" t="s">
         <v>45</v>
@@ -2603,13 +2616,13 @@
         <v>138</v>
       </c>
       <c r="B112">
-        <v>92438</v>
+        <v>41539</v>
       </c>
       <c r="C112">
         <v>3000</v>
       </c>
       <c r="D112">
-        <v>4624163</v>
+        <v>4570111</v>
       </c>
       <c r="E112" t="s">
         <v>45</v>
@@ -2620,13 +2633,13 @@
         <v>138</v>
       </c>
       <c r="B113">
-        <v>91405</v>
+        <v>92438</v>
       </c>
       <c r="C113">
         <v>3000</v>
       </c>
       <c r="D113">
-        <v>4613196</v>
+        <v>4624163</v>
       </c>
       <c r="E113" t="s">
         <v>45</v>
@@ -2634,19 +2647,19 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="B114">
-        <v>3024</v>
+        <v>91405</v>
       </c>
       <c r="C114">
         <v>3000</v>
       </c>
       <c r="D114">
-        <v>6099189</v>
+        <v>4613196</v>
       </c>
       <c r="E114" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -2654,13 +2667,13 @@
         <v>151</v>
       </c>
       <c r="B115">
-        <v>3023</v>
+        <v>3024</v>
       </c>
       <c r="C115">
         <v>3000</v>
       </c>
       <c r="D115">
-        <v>4655080</v>
+        <v>6099189</v>
       </c>
       <c r="E115" t="s">
         <v>51</v>
@@ -2671,13 +2684,13 @@
         <v>151</v>
       </c>
       <c r="B116">
-        <v>3623</v>
+        <v>3023</v>
       </c>
       <c r="C116">
         <v>3000</v>
       </c>
       <c r="D116">
-        <v>6069257</v>
+        <v>4655080</v>
       </c>
       <c r="E116" t="s">
         <v>51</v>
@@ -2688,13 +2701,13 @@
         <v>151</v>
       </c>
       <c r="B117">
-        <v>3666</v>
+        <v>3623</v>
       </c>
       <c r="C117">
         <v>3000</v>
       </c>
       <c r="D117">
-        <v>6099187</v>
+        <v>6069257</v>
       </c>
       <c r="E117" t="s">
         <v>51</v>
@@ -2705,13 +2718,13 @@
         <v>151</v>
       </c>
       <c r="B118">
-        <v>3022</v>
+        <v>3666</v>
       </c>
       <c r="C118">
         <v>3000</v>
       </c>
       <c r="D118">
-        <v>6186823</v>
+        <v>6099187</v>
       </c>
       <c r="E118" t="s">
         <v>51</v>
@@ -2722,13 +2735,13 @@
         <v>151</v>
       </c>
       <c r="B119">
-        <v>3021</v>
+        <v>3022</v>
       </c>
       <c r="C119">
         <v>3000</v>
       </c>
       <c r="D119">
-        <v>6184348</v>
+        <v>6186823</v>
       </c>
       <c r="E119" t="s">
         <v>51</v>
@@ -2739,13 +2752,13 @@
         <v>151</v>
       </c>
       <c r="B120">
-        <v>3020</v>
+        <v>3021</v>
       </c>
       <c r="C120">
         <v>3000</v>
       </c>
       <c r="D120">
-        <v>6249817</v>
+        <v>6184348</v>
       </c>
       <c r="E120" t="s">
         <v>51</v>
@@ -2756,13 +2769,13 @@
         <v>151</v>
       </c>
       <c r="B121">
-        <v>3795</v>
+        <v>3020</v>
       </c>
       <c r="C121">
         <v>3000</v>
       </c>
       <c r="D121">
-        <v>6194726</v>
+        <v>6249817</v>
       </c>
       <c r="E121" t="s">
         <v>51</v>
@@ -2773,13 +2786,13 @@
         <v>151</v>
       </c>
       <c r="B122">
-        <v>3034</v>
+        <v>3795</v>
       </c>
       <c r="C122">
-        <v>0</v>
-      </c>
-      <c r="D122" s="1">
-        <v>4155258</v>
+        <v>3000</v>
+      </c>
+      <c r="D122">
+        <v>6194726</v>
       </c>
       <c r="E122" t="s">
         <v>51</v>
@@ -2790,13 +2803,13 @@
         <v>151</v>
       </c>
       <c r="B123">
-        <v>3031</v>
+        <v>3034</v>
       </c>
       <c r="C123">
-        <v>3000</v>
-      </c>
-      <c r="D123">
-        <v>6227073</v>
+        <v>0</v>
+      </c>
+      <c r="D123" s="1">
+        <v>4155258</v>
       </c>
       <c r="E123" t="s">
         <v>51</v>
@@ -2807,13 +2820,13 @@
         <v>151</v>
       </c>
       <c r="B124">
-        <v>3958</v>
+        <v>3031</v>
       </c>
       <c r="C124">
         <v>3000</v>
       </c>
       <c r="D124">
-        <v>6186830</v>
+        <v>6227073</v>
       </c>
       <c r="E124" t="s">
         <v>51</v>
@@ -2824,13 +2837,13 @@
         <v>151</v>
       </c>
       <c r="B125">
-        <v>3036</v>
+        <v>3958</v>
       </c>
       <c r="C125">
-        <v>0</v>
-      </c>
-      <c r="D125" s="1">
-        <v>4595790</v>
+        <v>3000</v>
+      </c>
+      <c r="D125">
+        <v>6186830</v>
       </c>
       <c r="E125" t="s">
         <v>51</v>
@@ -2841,13 +2854,13 @@
         <v>151</v>
       </c>
       <c r="B126">
-        <v>3028</v>
+        <v>3036</v>
       </c>
       <c r="C126">
-        <v>3000</v>
-      </c>
-      <c r="D126">
-        <v>4266897</v>
+        <v>0</v>
+      </c>
+      <c r="D126" s="1">
+        <v>4595790</v>
       </c>
       <c r="E126" t="s">
         <v>51</v>
@@ -2858,13 +2871,13 @@
         <v>151</v>
       </c>
       <c r="B127">
-        <v>3027</v>
+        <v>3028</v>
       </c>
       <c r="C127">
         <v>3000</v>
       </c>
       <c r="D127">
-        <v>6109751</v>
+        <v>4266897</v>
       </c>
       <c r="E127" t="s">
         <v>51</v>
@@ -2875,13 +2888,13 @@
         <v>151</v>
       </c>
       <c r="B128">
-        <v>41539</v>
+        <v>3027</v>
       </c>
       <c r="C128">
-        <v>0</v>
-      </c>
-      <c r="D128" s="1">
-        <v>4158307</v>
+        <v>3000</v>
+      </c>
+      <c r="D128">
+        <v>6109751</v>
       </c>
       <c r="E128" t="s">
         <v>51</v>
@@ -2889,19 +2902,19 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="B129">
-        <v>3024</v>
+        <v>41539</v>
       </c>
       <c r="C129">
         <v>0</v>
       </c>
       <c r="D129" s="1">
-        <v>4184108</v>
+        <v>4158307</v>
       </c>
       <c r="E129" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -2909,13 +2922,13 @@
         <v>140</v>
       </c>
       <c r="B130">
-        <v>3023</v>
+        <v>3024</v>
       </c>
       <c r="C130">
-        <v>3000</v>
-      </c>
-      <c r="D130">
-        <v>4528981</v>
+        <v>0</v>
+      </c>
+      <c r="D130" s="1">
+        <v>4184108</v>
       </c>
       <c r="E130" t="s">
         <v>53</v>
@@ -2926,13 +2939,13 @@
         <v>140</v>
       </c>
       <c r="B131">
-        <v>3623</v>
+        <v>3023</v>
       </c>
       <c r="C131">
         <v>3000</v>
       </c>
       <c r="D131">
-        <v>4177735</v>
+        <v>4528981</v>
       </c>
       <c r="E131" t="s">
         <v>53</v>
@@ -2943,13 +2956,13 @@
         <v>140</v>
       </c>
       <c r="B132">
-        <v>3710</v>
+        <v>3623</v>
       </c>
       <c r="C132">
         <v>3000</v>
       </c>
       <c r="D132">
-        <v>4502089</v>
+        <v>4177735</v>
       </c>
       <c r="E132" t="s">
         <v>53</v>
@@ -2960,13 +2973,13 @@
         <v>140</v>
       </c>
       <c r="B133">
-        <v>3666</v>
+        <v>3710</v>
       </c>
       <c r="C133">
         <v>3000</v>
       </c>
       <c r="D133">
-        <v>4508313</v>
+        <v>4502089</v>
       </c>
       <c r="E133" t="s">
         <v>53</v>
@@ -2977,13 +2990,13 @@
         <v>140</v>
       </c>
       <c r="B134">
-        <v>3460</v>
+        <v>3666</v>
       </c>
       <c r="C134">
         <v>3000</v>
       </c>
       <c r="D134">
-        <v>6250216</v>
+        <v>4508313</v>
       </c>
       <c r="E134" t="s">
         <v>53</v>
@@ -2994,13 +3007,13 @@
         <v>140</v>
       </c>
       <c r="B135">
-        <v>4477</v>
+        <v>3460</v>
       </c>
       <c r="C135">
         <v>3000</v>
       </c>
       <c r="D135">
-        <v>6200663</v>
+        <v>6250216</v>
       </c>
       <c r="E135" t="s">
         <v>53</v>
@@ -3011,13 +3024,13 @@
         <v>140</v>
       </c>
       <c r="B136">
-        <v>3022</v>
+        <v>4477</v>
       </c>
       <c r="C136">
         <v>3000</v>
       </c>
       <c r="D136">
-        <v>6037890</v>
+        <v>6200663</v>
       </c>
       <c r="E136" t="s">
         <v>53</v>
@@ -3028,48 +3041,48 @@
         <v>140</v>
       </c>
       <c r="B137">
-        <v>3021</v>
+        <v>3022</v>
       </c>
       <c r="C137">
         <v>3000</v>
       </c>
       <c r="D137">
-        <v>4530028</v>
+        <v>6037890</v>
       </c>
       <c r="E137" t="s">
         <v>53</v>
       </c>
-      <c r="F137" s="1"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>140</v>
       </c>
       <c r="B138">
-        <v>3020</v>
+        <v>3021</v>
       </c>
       <c r="C138">
         <v>3000</v>
       </c>
       <c r="D138">
-        <v>4667595</v>
+        <v>4530028</v>
       </c>
       <c r="E138" t="s">
         <v>53</v>
       </c>
+      <c r="F138" s="1"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>140</v>
       </c>
       <c r="B139">
-        <v>3795</v>
+        <v>3020</v>
       </c>
       <c r="C139">
-        <v>0</v>
-      </c>
-      <c r="D139" s="1">
-        <v>6097420</v>
+        <v>3000</v>
+      </c>
+      <c r="D139">
+        <v>4667595</v>
       </c>
       <c r="E139" t="s">
         <v>53</v>
@@ -3080,13 +3093,13 @@
         <v>140</v>
       </c>
       <c r="B140">
-        <v>3034</v>
+        <v>3795</v>
       </c>
       <c r="C140">
-        <v>3000</v>
-      </c>
-      <c r="D140">
-        <v>6027627</v>
+        <v>0</v>
+      </c>
+      <c r="D140" s="1">
+        <v>6097420</v>
       </c>
       <c r="E140" t="s">
         <v>53</v>
@@ -3097,13 +3110,13 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>2445</v>
+        <v>3034</v>
       </c>
       <c r="C141">
         <v>3000</v>
       </c>
       <c r="D141">
-        <v>6218082</v>
+        <v>6027627</v>
       </c>
       <c r="E141" t="s">
         <v>53</v>
@@ -3114,48 +3127,48 @@
         <v>140</v>
       </c>
       <c r="B142">
-        <v>91988</v>
+        <v>2445</v>
       </c>
       <c r="C142">
         <v>3000</v>
       </c>
       <c r="D142">
-        <v>6186638</v>
+        <v>6218082</v>
       </c>
       <c r="E142" t="s">
         <v>53</v>
       </c>
-      <c r="G142" s="1"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>140</v>
       </c>
       <c r="B143">
-        <v>4282</v>
+        <v>91988</v>
       </c>
       <c r="C143">
         <v>3000</v>
       </c>
       <c r="D143">
-        <v>6120642</v>
+        <v>6186638</v>
       </c>
       <c r="E143" t="s">
         <v>53</v>
       </c>
+      <c r="G143" s="1"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>140</v>
       </c>
       <c r="B144">
-        <v>3031</v>
+        <v>4282</v>
       </c>
       <c r="C144">
         <v>3000</v>
       </c>
       <c r="D144">
-        <v>6027625</v>
+        <v>6120642</v>
       </c>
       <c r="E144" t="s">
         <v>53</v>
@@ -3166,13 +3179,13 @@
         <v>140</v>
       </c>
       <c r="B145">
-        <v>3032</v>
+        <v>3031</v>
       </c>
       <c r="C145">
         <v>3000</v>
       </c>
       <c r="D145">
-        <v>6037887</v>
+        <v>6027625</v>
       </c>
       <c r="E145" t="s">
         <v>53</v>
@@ -3183,13 +3196,13 @@
         <v>140</v>
       </c>
       <c r="B146">
-        <v>3029</v>
+        <v>3032</v>
       </c>
       <c r="C146">
         <v>3000</v>
       </c>
       <c r="D146">
-        <v>6270715</v>
+        <v>6037887</v>
       </c>
       <c r="E146" t="s">
         <v>53</v>
@@ -3200,13 +3213,13 @@
         <v>140</v>
       </c>
       <c r="B147">
-        <v>3958</v>
+        <v>3029</v>
       </c>
       <c r="C147">
         <v>3000</v>
       </c>
       <c r="D147">
-        <v>6106692</v>
+        <v>6270715</v>
       </c>
       <c r="E147" t="s">
         <v>53</v>
@@ -3217,49 +3230,49 @@
         <v>140</v>
       </c>
       <c r="B148">
-        <v>3036</v>
+        <v>3958</v>
       </c>
       <c r="C148">
         <v>3000</v>
       </c>
       <c r="D148">
-        <v>6146302</v>
+        <v>6106692</v>
       </c>
       <c r="E148" t="s">
         <v>53</v>
       </c>
-      <c r="F148" s="1"/>
-      <c r="G148" s="1"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>140</v>
       </c>
       <c r="B149">
-        <v>3033</v>
+        <v>3036</v>
       </c>
       <c r="C149">
         <v>3000</v>
       </c>
       <c r="D149">
-        <v>6200659</v>
+        <v>6146302</v>
       </c>
       <c r="E149" t="s">
         <v>53</v>
       </c>
+      <c r="F149" s="1"/>
+      <c r="G149" s="1"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>140</v>
       </c>
       <c r="B150">
-        <v>3456</v>
+        <v>3033</v>
       </c>
       <c r="C150">
-        <v>0</v>
-      </c>
-      <c r="D150" s="1">
-        <v>4595163</v>
+        <v>3000</v>
+      </c>
+      <c r="D150">
+        <v>6200659</v>
       </c>
       <c r="E150" t="s">
         <v>53</v>
@@ -3267,19 +3280,19 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B151">
-        <v>3024</v>
+        <v>3456</v>
       </c>
       <c r="C151">
-        <v>3000</v>
-      </c>
-      <c r="D151">
-        <v>6055169</v>
+        <v>0</v>
+      </c>
+      <c r="D151" s="1">
+        <v>4595163</v>
       </c>
       <c r="E151" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
@@ -3287,13 +3300,13 @@
         <v>141</v>
       </c>
       <c r="B152">
-        <v>3023</v>
+        <v>3024</v>
       </c>
       <c r="C152">
         <v>3000</v>
       </c>
       <c r="D152">
-        <v>6013102</v>
+        <v>6055169</v>
       </c>
       <c r="E152" t="s">
         <v>49</v>
@@ -3304,66 +3317,65 @@
         <v>141</v>
       </c>
       <c r="B153">
-        <v>3623</v>
+        <v>3023</v>
       </c>
       <c r="C153">
         <v>3000</v>
       </c>
       <c r="D153">
-        <v>6013975</v>
+        <v>6013102</v>
       </c>
       <c r="E153" t="s">
         <v>49</v>
       </c>
-      <c r="G153" s="1"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>141</v>
       </c>
       <c r="B154">
-        <v>3710</v>
+        <v>3623</v>
       </c>
       <c r="C154">
         <v>3000</v>
       </c>
       <c r="D154">
-        <v>6020923</v>
+        <v>6013975</v>
       </c>
       <c r="E154" t="s">
         <v>49</v>
       </c>
+      <c r="G154" s="1"/>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>141</v>
       </c>
       <c r="B155">
-        <v>3666</v>
+        <v>3710</v>
       </c>
       <c r="C155">
         <v>3000</v>
       </c>
       <c r="D155">
-        <v>4245566</v>
+        <v>6020923</v>
       </c>
       <c r="E155" t="s">
         <v>49</v>
       </c>
-      <c r="G155" s="1"/>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>141</v>
       </c>
       <c r="B156">
-        <v>3460</v>
+        <v>3666</v>
       </c>
       <c r="C156">
-        <v>0</v>
-      </c>
-      <c r="D156" s="1">
-        <v>4264408</v>
+        <v>3000</v>
+      </c>
+      <c r="D156">
+        <v>4245566</v>
       </c>
       <c r="E156" t="s">
         <v>49</v>
@@ -3375,13 +3387,13 @@
         <v>141</v>
       </c>
       <c r="B157">
-        <v>3021</v>
+        <v>3460</v>
       </c>
       <c r="C157">
-        <v>3000</v>
-      </c>
-      <c r="D157">
-        <v>4650244</v>
+        <v>0</v>
+      </c>
+      <c r="D157" s="1">
+        <v>4264408</v>
       </c>
       <c r="E157" t="s">
         <v>49</v>
@@ -3393,118 +3405,118 @@
         <v>141</v>
       </c>
       <c r="B158">
-        <v>3020</v>
+        <v>3021</v>
       </c>
       <c r="C158">
         <v>3000</v>
       </c>
       <c r="D158">
-        <v>4586057</v>
+        <v>4650244</v>
       </c>
       <c r="E158" t="s">
         <v>49</v>
       </c>
+      <c r="G158" s="1"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>141</v>
       </c>
       <c r="B159">
-        <v>3795</v>
+        <v>3020</v>
       </c>
       <c r="C159">
-        <v>0</v>
-      </c>
-      <c r="D159" s="1">
-        <v>4245554</v>
+        <v>3000</v>
+      </c>
+      <c r="D159">
+        <v>4586057</v>
       </c>
       <c r="E159" t="s">
         <v>49</v>
       </c>
-      <c r="G159" s="1"/>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>141</v>
       </c>
       <c r="B160">
-        <v>3034</v>
+        <v>3795</v>
       </c>
       <c r="C160">
-        <v>3000</v>
-      </c>
-      <c r="D160">
-        <v>6174940</v>
+        <v>0</v>
+      </c>
+      <c r="D160" s="1">
+        <v>4245554</v>
       </c>
       <c r="E160" t="s">
         <v>49</v>
       </c>
+      <c r="G160" s="1"/>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>141</v>
       </c>
       <c r="B161">
-        <v>4282</v>
+        <v>3034</v>
       </c>
       <c r="C161">
-        <v>0</v>
-      </c>
-      <c r="D161" s="1">
-        <v>4583692</v>
+        <v>3000</v>
+      </c>
+      <c r="D161">
+        <v>6174940</v>
       </c>
       <c r="E161" t="s">
         <v>49</v>
       </c>
-      <c r="G161" s="1"/>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>141</v>
       </c>
       <c r="B162">
-        <v>3032</v>
+        <v>4282</v>
       </c>
       <c r="C162">
         <v>0</v>
       </c>
       <c r="D162" s="1">
-        <v>4252317</v>
+        <v>4583692</v>
       </c>
       <c r="E162" t="s">
         <v>49</v>
       </c>
+      <c r="G162" s="1"/>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>141</v>
       </c>
       <c r="B163">
-        <v>3035</v>
+        <v>3032</v>
       </c>
       <c r="C163">
         <v>0</v>
       </c>
       <c r="D163" s="1">
-        <v>4505051</v>
+        <v>4252317</v>
       </c>
       <c r="E163" t="s">
         <v>49</v>
       </c>
-      <c r="F163" s="1"/>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>141</v>
       </c>
       <c r="B164">
-        <v>3030</v>
+        <v>3035</v>
       </c>
       <c r="C164">
         <v>0</v>
       </c>
       <c r="D164" s="1">
-        <v>4295024</v>
+        <v>4505051</v>
       </c>
       <c r="E164" t="s">
         <v>49</v>
@@ -3516,13 +3528,13 @@
         <v>141</v>
       </c>
       <c r="B165">
-        <v>3029</v>
+        <v>3030</v>
       </c>
       <c r="C165">
-        <v>3000</v>
-      </c>
-      <c r="D165">
-        <v>4292461</v>
+        <v>0</v>
+      </c>
+      <c r="D165" s="1">
+        <v>4295024</v>
       </c>
       <c r="E165" t="s">
         <v>49</v>
@@ -3534,48 +3546,49 @@
         <v>141</v>
       </c>
       <c r="B166">
-        <v>3958</v>
+        <v>3029</v>
       </c>
       <c r="C166">
-        <v>0</v>
-      </c>
-      <c r="D166" s="1">
-        <v>6186831</v>
+        <v>3000</v>
+      </c>
+      <c r="D166">
+        <v>4292461</v>
       </c>
       <c r="E166" t="s">
         <v>49</v>
       </c>
-      <c r="G166" s="1"/>
+      <c r="F166" s="1"/>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>141</v>
       </c>
       <c r="B167">
-        <v>3033</v>
+        <v>3958</v>
       </c>
       <c r="C167">
         <v>0</v>
       </c>
       <c r="D167" s="1">
-        <v>4549214</v>
+        <v>6186831</v>
       </c>
       <c r="E167" t="s">
         <v>49</v>
       </c>
+      <c r="G167" s="1"/>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>141</v>
       </c>
       <c r="B168">
-        <v>3028</v>
+        <v>3033</v>
       </c>
       <c r="C168">
-        <v>3000</v>
-      </c>
-      <c r="D168">
-        <v>4264818</v>
+        <v>0</v>
+      </c>
+      <c r="D168" s="1">
+        <v>4549214</v>
       </c>
       <c r="E168" t="s">
         <v>49</v>
@@ -3586,13 +3599,13 @@
         <v>141</v>
       </c>
       <c r="B169">
-        <v>92438</v>
+        <v>3028</v>
       </c>
       <c r="C169">
-        <v>0</v>
-      </c>
-      <c r="D169" s="1">
-        <v>6001820</v>
+        <v>3000</v>
+      </c>
+      <c r="D169">
+        <v>4264818</v>
       </c>
       <c r="E169" t="s">
         <v>49</v>
@@ -3600,19 +3613,19 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="B170">
-        <v>3024</v>
+        <v>92438</v>
       </c>
       <c r="C170">
-        <v>3000</v>
-      </c>
-      <c r="D170">
-        <v>4539114</v>
+        <v>0</v>
+      </c>
+      <c r="D170" s="1">
+        <v>6001820</v>
       </c>
       <c r="E170" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
@@ -3620,13 +3633,13 @@
         <v>154</v>
       </c>
       <c r="B171">
-        <v>3023</v>
+        <v>3024</v>
       </c>
       <c r="C171">
         <v>3000</v>
       </c>
       <c r="D171">
-        <v>4539097</v>
+        <v>4539114</v>
       </c>
       <c r="E171" t="s">
         <v>52</v>
@@ -3637,13 +3650,13 @@
         <v>154</v>
       </c>
       <c r="B172">
-        <v>3623</v>
+        <v>3023</v>
       </c>
       <c r="C172">
         <v>3000</v>
       </c>
       <c r="D172">
-        <v>4539076</v>
+        <v>4539097</v>
       </c>
       <c r="E172" t="s">
         <v>52</v>
@@ -3654,13 +3667,13 @@
         <v>154</v>
       </c>
       <c r="B173">
-        <v>3710</v>
+        <v>3623</v>
       </c>
       <c r="C173">
         <v>3000</v>
       </c>
       <c r="D173">
-        <v>4539061</v>
+        <v>4539076</v>
       </c>
       <c r="E173" t="s">
         <v>52</v>
@@ -3671,13 +3684,13 @@
         <v>154</v>
       </c>
       <c r="B174">
-        <v>3666</v>
+        <v>3710</v>
       </c>
       <c r="C174">
         <v>3000</v>
       </c>
       <c r="D174">
-        <v>4539062</v>
+        <v>4539061</v>
       </c>
       <c r="E174" t="s">
         <v>52</v>
@@ -3688,13 +3701,13 @@
         <v>154</v>
       </c>
       <c r="B175">
-        <v>3460</v>
+        <v>3666</v>
       </c>
       <c r="C175">
         <v>3000</v>
       </c>
       <c r="D175">
-        <v>4541507</v>
+        <v>4539062</v>
       </c>
       <c r="E175" t="s">
         <v>52</v>
@@ -3705,13 +3718,13 @@
         <v>154</v>
       </c>
       <c r="B176">
-        <v>4477</v>
+        <v>3460</v>
       </c>
       <c r="C176">
         <v>3000</v>
       </c>
       <c r="D176">
-        <v>6037995</v>
+        <v>4541507</v>
       </c>
       <c r="E176" t="s">
         <v>52</v>
@@ -3722,13 +3735,13 @@
         <v>154</v>
       </c>
       <c r="B177">
-        <v>60479</v>
+        <v>4477</v>
       </c>
       <c r="C177">
         <v>3000</v>
       </c>
       <c r="D177">
-        <v>6253142</v>
+        <v>6037995</v>
       </c>
       <c r="E177" t="s">
         <v>52</v>
@@ -3739,13 +3752,13 @@
         <v>154</v>
       </c>
       <c r="B178">
-        <v>3022</v>
+        <v>60479</v>
       </c>
       <c r="C178">
         <v>3000</v>
       </c>
       <c r="D178">
-        <v>4585479</v>
+        <v>6253142</v>
       </c>
       <c r="E178" t="s">
         <v>52</v>
@@ -3756,13 +3769,13 @@
         <v>154</v>
       </c>
       <c r="B179">
-        <v>3021</v>
+        <v>3022</v>
       </c>
       <c r="C179">
-        <v>0</v>
-      </c>
-      <c r="D179" s="1">
-        <v>4177047</v>
+        <v>3000</v>
+      </c>
+      <c r="D179">
+        <v>4585479</v>
       </c>
       <c r="E179" t="s">
         <v>52</v>
@@ -3773,13 +3786,13 @@
         <v>154</v>
       </c>
       <c r="B180">
-        <v>3020</v>
+        <v>3021</v>
       </c>
       <c r="C180">
-        <v>3000</v>
-      </c>
-      <c r="D180">
-        <v>4539071</v>
+        <v>0</v>
+      </c>
+      <c r="D180" s="1">
+        <v>4177047</v>
       </c>
       <c r="E180" t="s">
         <v>52</v>
@@ -3790,13 +3803,13 @@
         <v>154</v>
       </c>
       <c r="B181">
-        <v>3034</v>
+        <v>3020</v>
       </c>
       <c r="C181">
         <v>3000</v>
       </c>
       <c r="D181">
-        <v>6152321</v>
+        <v>4539071</v>
       </c>
       <c r="E181" t="s">
         <v>52</v>
@@ -3807,13 +3820,13 @@
         <v>154</v>
       </c>
       <c r="B182">
-        <v>3832</v>
+        <v>3034</v>
       </c>
       <c r="C182">
-        <v>0</v>
-      </c>
-      <c r="D182" s="1">
-        <v>4223849</v>
+        <v>3000</v>
+      </c>
+      <c r="D182">
+        <v>6152321</v>
       </c>
       <c r="E182" t="s">
         <v>52</v>
@@ -3824,13 +3837,13 @@
         <v>154</v>
       </c>
       <c r="B183">
-        <v>2445</v>
+        <v>3832</v>
       </c>
       <c r="C183">
         <v>0</v>
       </c>
       <c r="D183" s="1">
-        <v>4279712</v>
+        <v>4223849</v>
       </c>
       <c r="E183" t="s">
         <v>52</v>
@@ -3841,13 +3854,13 @@
         <v>154</v>
       </c>
       <c r="B184">
-        <v>3031</v>
+        <v>2445</v>
       </c>
       <c r="C184">
-        <v>3000</v>
-      </c>
-      <c r="D184">
-        <v>6134368</v>
+        <v>0</v>
+      </c>
+      <c r="D184" s="1">
+        <v>4279712</v>
       </c>
       <c r="E184" t="s">
         <v>52</v>
@@ -3858,13 +3871,13 @@
         <v>154</v>
       </c>
       <c r="B185">
-        <v>3032</v>
+        <v>3031</v>
       </c>
       <c r="C185">
-        <v>0</v>
-      </c>
-      <c r="D185" s="1">
-        <v>6020122</v>
+        <v>3000</v>
+      </c>
+      <c r="D185">
+        <v>6134368</v>
       </c>
       <c r="E185" t="s">
         <v>52</v>
@@ -3875,13 +3888,13 @@
         <v>154</v>
       </c>
       <c r="B186">
-        <v>3035</v>
+        <v>3032</v>
       </c>
       <c r="C186">
         <v>0</v>
       </c>
       <c r="D186" s="1">
-        <v>4256094</v>
+        <v>6020122</v>
       </c>
       <c r="E186" t="s">
         <v>52</v>
@@ -3892,13 +3905,13 @@
         <v>154</v>
       </c>
       <c r="B187">
-        <v>3030</v>
+        <v>3035</v>
       </c>
       <c r="C187">
-        <v>3000</v>
-      </c>
-      <c r="D187">
-        <v>6186106</v>
+        <v>0</v>
+      </c>
+      <c r="D187" s="1">
+        <v>4256094</v>
       </c>
       <c r="E187" t="s">
         <v>52</v>
@@ -3909,13 +3922,13 @@
         <v>154</v>
       </c>
       <c r="B188">
-        <v>3029</v>
+        <v>3030</v>
       </c>
       <c r="C188">
-        <v>0</v>
-      </c>
-      <c r="D188" s="1">
-        <v>4164218</v>
+        <v>3000</v>
+      </c>
+      <c r="D188">
+        <v>6186106</v>
       </c>
       <c r="E188" t="s">
         <v>52</v>
@@ -3926,13 +3939,13 @@
         <v>154</v>
       </c>
       <c r="B189">
-        <v>3958</v>
+        <v>3029</v>
       </c>
       <c r="C189">
-        <v>3000</v>
-      </c>
-      <c r="D189">
-        <v>6173945</v>
+        <v>0</v>
+      </c>
+      <c r="D189" s="1">
+        <v>4164218</v>
       </c>
       <c r="E189" t="s">
         <v>52</v>
@@ -3943,13 +3956,13 @@
         <v>154</v>
       </c>
       <c r="B190">
-        <v>3036</v>
+        <v>3958</v>
       </c>
       <c r="C190">
         <v>3000</v>
       </c>
       <c r="D190">
-        <v>6028115</v>
+        <v>6173945</v>
       </c>
       <c r="E190" t="s">
         <v>52</v>
@@ -3960,13 +3973,13 @@
         <v>154</v>
       </c>
       <c r="B191">
-        <v>3033</v>
+        <v>3036</v>
       </c>
       <c r="C191">
-        <v>0</v>
-      </c>
-      <c r="D191" s="1">
-        <v>6052874</v>
+        <v>3000</v>
+      </c>
+      <c r="D191">
+        <v>6028115</v>
       </c>
       <c r="E191" t="s">
         <v>52</v>
@@ -3977,13 +3990,13 @@
         <v>154</v>
       </c>
       <c r="B192">
-        <v>3028</v>
+        <v>3033</v>
       </c>
       <c r="C192">
-        <v>3000</v>
-      </c>
-      <c r="D192">
-        <v>6212076</v>
+        <v>0</v>
+      </c>
+      <c r="D192" s="1">
+        <v>6052874</v>
       </c>
       <c r="E192" t="s">
         <v>52</v>
@@ -3994,13 +4007,13 @@
         <v>154</v>
       </c>
       <c r="B193">
-        <v>3456</v>
+        <v>3028</v>
       </c>
       <c r="C193">
-        <v>0</v>
-      </c>
-      <c r="D193" s="1">
-        <v>4541385</v>
+        <v>3000</v>
+      </c>
+      <c r="D193">
+        <v>6212076</v>
       </c>
       <c r="E193" t="s">
         <v>52</v>
@@ -4011,13 +4024,13 @@
         <v>154</v>
       </c>
       <c r="B194">
-        <v>3027</v>
+        <v>3456</v>
       </c>
       <c r="C194">
         <v>0</v>
       </c>
       <c r="D194" s="1">
-        <v>4264807</v>
+        <v>4541385</v>
       </c>
       <c r="E194" t="s">
         <v>52</v>
@@ -4028,13 +4041,13 @@
         <v>154</v>
       </c>
       <c r="B195">
-        <v>41539</v>
+        <v>3027</v>
       </c>
       <c r="C195">
         <v>0</v>
       </c>
       <c r="D195" s="1">
-        <v>4262018</v>
+        <v>4264807</v>
       </c>
       <c r="E195" t="s">
         <v>52</v>
@@ -4042,19 +4055,19 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196">
-        <v>191</v>
+        <v>154</v>
       </c>
       <c r="B196">
-        <v>3024</v>
+        <v>41539</v>
       </c>
       <c r="C196">
-        <v>3000</v>
-      </c>
-      <c r="D196">
-        <v>6073040</v>
+        <v>0</v>
+      </c>
+      <c r="D196" s="1">
+        <v>4262018</v>
       </c>
       <c r="E196" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -4062,13 +4075,13 @@
         <v>191</v>
       </c>
       <c r="B197">
-        <v>3023</v>
+        <v>3024</v>
       </c>
       <c r="C197">
         <v>3000</v>
       </c>
       <c r="D197">
-        <v>6028736</v>
+        <v>6073040</v>
       </c>
       <c r="E197" t="s">
         <v>54</v>
@@ -4079,13 +4092,13 @@
         <v>191</v>
       </c>
       <c r="B198">
-        <v>3623</v>
+        <v>3023</v>
       </c>
       <c r="C198">
         <v>3000</v>
       </c>
       <c r="D198">
-        <v>6073042</v>
+        <v>6028736</v>
       </c>
       <c r="E198" t="s">
         <v>54</v>
@@ -4096,13 +4109,13 @@
         <v>191</v>
       </c>
       <c r="B199">
-        <v>3710</v>
+        <v>3623</v>
       </c>
       <c r="C199">
         <v>3000</v>
       </c>
       <c r="D199">
-        <v>6020073</v>
+        <v>6073042</v>
       </c>
       <c r="E199" t="s">
         <v>54</v>
@@ -4113,13 +4126,13 @@
         <v>191</v>
       </c>
       <c r="B200">
-        <v>3666</v>
+        <v>3710</v>
       </c>
       <c r="C200">
         <v>3000</v>
       </c>
       <c r="D200">
-        <v>6020074</v>
+        <v>6020073</v>
       </c>
       <c r="E200" t="s">
         <v>54</v>
@@ -4130,13 +4143,13 @@
         <v>191</v>
       </c>
       <c r="B201">
-        <v>3460</v>
+        <v>3666</v>
       </c>
       <c r="C201">
         <v>3000</v>
       </c>
       <c r="D201">
-        <v>6192205</v>
+        <v>6020074</v>
       </c>
       <c r="E201" t="s">
         <v>54</v>
@@ -4147,13 +4160,13 @@
         <v>191</v>
       </c>
       <c r="B202">
-        <v>3022</v>
+        <v>3460</v>
       </c>
       <c r="C202">
         <v>3000</v>
       </c>
       <c r="D202">
-        <v>6003033</v>
+        <v>6192205</v>
       </c>
       <c r="E202" t="s">
         <v>54</v>
@@ -4164,13 +4177,13 @@
         <v>191</v>
       </c>
       <c r="B203">
-        <v>3021</v>
+        <v>3022</v>
       </c>
       <c r="C203">
         <v>3000</v>
       </c>
       <c r="D203">
-        <v>6097503</v>
+        <v>6003033</v>
       </c>
       <c r="E203" t="s">
         <v>54</v>
@@ -4181,13 +4194,13 @@
         <v>191</v>
       </c>
       <c r="B204">
-        <v>3020</v>
+        <v>3021</v>
       </c>
       <c r="C204">
         <v>3000</v>
       </c>
       <c r="D204">
-        <v>6097511</v>
+        <v>6097503</v>
       </c>
       <c r="E204" t="s">
         <v>54</v>
@@ -4198,13 +4211,13 @@
         <v>191</v>
       </c>
       <c r="B205">
-        <v>3795</v>
+        <v>3020</v>
       </c>
       <c r="C205">
         <v>3000</v>
       </c>
       <c r="D205">
-        <v>6097509</v>
+        <v>6097511</v>
       </c>
       <c r="E205" t="s">
         <v>54</v>
@@ -4215,13 +4228,13 @@
         <v>191</v>
       </c>
       <c r="B206">
-        <v>3034</v>
+        <v>3795</v>
       </c>
       <c r="C206">
         <v>3000</v>
       </c>
       <c r="D206">
-        <v>6133817</v>
+        <v>6097509</v>
       </c>
       <c r="E206" t="s">
         <v>54</v>
@@ -4232,13 +4245,13 @@
         <v>191</v>
       </c>
       <c r="B207">
-        <v>4282</v>
+        <v>3034</v>
       </c>
       <c r="C207">
-        <v>0</v>
-      </c>
-      <c r="D207" s="1">
-        <v>6172377</v>
+        <v>3000</v>
+      </c>
+      <c r="D207">
+        <v>6133817</v>
       </c>
       <c r="E207" t="s">
         <v>54</v>
@@ -4249,13 +4262,13 @@
         <v>191</v>
       </c>
       <c r="B208">
-        <v>3031</v>
+        <v>4282</v>
       </c>
       <c r="C208">
         <v>0</v>
       </c>
-      <c r="D208">
-        <v>6093272</v>
+      <c r="D208" s="1">
+        <v>6172377</v>
       </c>
       <c r="E208" t="s">
         <v>54</v>
@@ -4266,13 +4279,13 @@
         <v>191</v>
       </c>
       <c r="B209">
-        <v>3032</v>
+        <v>3031</v>
       </c>
       <c r="C209">
         <v>0</v>
       </c>
-      <c r="D209" s="1">
-        <v>4243929</v>
+      <c r="D209">
+        <v>6093272</v>
       </c>
       <c r="E209" t="s">
         <v>54</v>
@@ -4283,13 +4296,13 @@
         <v>191</v>
       </c>
       <c r="B210">
-        <v>3456</v>
+        <v>3032</v>
       </c>
       <c r="C210">
         <v>0</v>
       </c>
       <c r="D210" s="1">
-        <v>6151065</v>
+        <v>4243929</v>
       </c>
       <c r="E210" t="s">
         <v>54</v>
@@ -4297,19 +4310,19 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B211">
-        <v>3024</v>
+        <v>3456</v>
       </c>
       <c r="C211">
-        <v>3000</v>
-      </c>
-      <c r="D211">
-        <v>4211399</v>
+        <v>0</v>
+      </c>
+      <c r="D211" s="1">
+        <v>6151065</v>
       </c>
       <c r="E211" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -4317,13 +4330,13 @@
         <v>194</v>
       </c>
       <c r="B212">
-        <v>3023</v>
+        <v>3024</v>
       </c>
       <c r="C212">
         <v>3000</v>
       </c>
       <c r="D212">
-        <v>4211398</v>
+        <v>4211399</v>
       </c>
       <c r="E212" t="s">
         <v>46</v>
@@ -4334,13 +4347,13 @@
         <v>194</v>
       </c>
       <c r="B213">
-        <v>3623</v>
+        <v>3023</v>
       </c>
       <c r="C213">
-        <v>0</v>
-      </c>
-      <c r="D213" s="1">
-        <v>4211429</v>
+        <v>3000</v>
+      </c>
+      <c r="D213">
+        <v>4211398</v>
       </c>
       <c r="E213" t="s">
         <v>46</v>
@@ -4351,13 +4364,13 @@
         <v>194</v>
       </c>
       <c r="B214">
-        <v>3710</v>
+        <v>3623</v>
       </c>
       <c r="C214">
-        <v>3000</v>
-      </c>
-      <c r="D214">
-        <v>4211445</v>
+        <v>0</v>
+      </c>
+      <c r="D214" s="1">
+        <v>4211429</v>
       </c>
       <c r="E214" t="s">
         <v>46</v>
@@ -4368,13 +4381,13 @@
         <v>194</v>
       </c>
       <c r="B215">
-        <v>3666</v>
+        <v>3710</v>
       </c>
       <c r="C215">
         <v>3000</v>
       </c>
       <c r="D215">
-        <v>4211438</v>
+        <v>4211445</v>
       </c>
       <c r="E215" t="s">
         <v>46</v>
@@ -4385,13 +4398,13 @@
         <v>194</v>
       </c>
       <c r="B216">
-        <v>3460</v>
+        <v>3666</v>
       </c>
       <c r="C216">
         <v>3000</v>
       </c>
       <c r="D216">
-        <v>4211425</v>
+        <v>4211438</v>
       </c>
       <c r="E216" t="s">
         <v>46</v>
@@ -4402,13 +4415,13 @@
         <v>194</v>
       </c>
       <c r="B217">
-        <v>4477</v>
+        <v>3460</v>
       </c>
       <c r="C217">
         <v>3000</v>
       </c>
       <c r="D217">
-        <v>4251149</v>
+        <v>4211425</v>
       </c>
       <c r="E217" t="s">
         <v>46</v>
@@ -4419,13 +4432,13 @@
         <v>194</v>
       </c>
       <c r="B218">
-        <v>60479</v>
+        <v>4477</v>
       </c>
       <c r="C218">
         <v>3000</v>
       </c>
       <c r="D218">
-        <v>4514846</v>
+        <v>4251149</v>
       </c>
       <c r="E218" t="s">
         <v>46</v>
@@ -4436,13 +4449,13 @@
         <v>194</v>
       </c>
       <c r="B219">
-        <v>3022</v>
+        <v>60479</v>
       </c>
       <c r="C219">
         <v>3000</v>
       </c>
       <c r="D219">
-        <v>4211397</v>
+        <v>4514846</v>
       </c>
       <c r="E219" t="s">
         <v>46</v>
@@ -4453,13 +4466,13 @@
         <v>194</v>
       </c>
       <c r="B220">
-        <v>3021</v>
+        <v>3022</v>
       </c>
       <c r="C220">
         <v>3000</v>
       </c>
       <c r="D220">
-        <v>4211396</v>
+        <v>4211397</v>
       </c>
       <c r="E220" t="s">
         <v>46</v>
@@ -4470,13 +4483,13 @@
         <v>194</v>
       </c>
       <c r="B221">
-        <v>3020</v>
+        <v>3021</v>
       </c>
       <c r="C221">
         <v>3000</v>
       </c>
       <c r="D221">
-        <v>4211395</v>
+        <v>4211396</v>
       </c>
       <c r="E221" t="s">
         <v>46</v>
@@ -4487,13 +4500,13 @@
         <v>194</v>
       </c>
       <c r="B222">
-        <v>3795</v>
+        <v>3020</v>
       </c>
       <c r="C222">
         <v>3000</v>
       </c>
       <c r="D222">
-        <v>4211452</v>
+        <v>4211395</v>
       </c>
       <c r="E222" t="s">
         <v>46</v>
@@ -4504,13 +4517,13 @@
         <v>194</v>
       </c>
       <c r="B223">
-        <v>3034</v>
+        <v>3795</v>
       </c>
       <c r="C223">
         <v>3000</v>
       </c>
       <c r="D223">
-        <v>4211406</v>
+        <v>4211452</v>
       </c>
       <c r="E223" t="s">
         <v>46</v>
@@ -4521,13 +4534,13 @@
         <v>194</v>
       </c>
       <c r="B224">
-        <v>3832</v>
+        <v>3034</v>
       </c>
       <c r="C224">
         <v>3000</v>
       </c>
       <c r="D224">
-        <v>4211462</v>
+        <v>4211406</v>
       </c>
       <c r="E224" t="s">
         <v>46</v>
@@ -4538,13 +4551,13 @@
         <v>194</v>
       </c>
       <c r="B225">
-        <v>2445</v>
+        <v>3832</v>
       </c>
       <c r="C225">
         <v>3000</v>
       </c>
       <c r="D225">
-        <v>4211360</v>
+        <v>4211462</v>
       </c>
       <c r="E225" t="s">
         <v>46</v>
@@ -4555,13 +4568,13 @@
         <v>194</v>
       </c>
       <c r="B226">
-        <v>91988</v>
+        <v>2445</v>
       </c>
       <c r="C226">
         <v>3000</v>
       </c>
       <c r="D226">
-        <v>4662161</v>
+        <v>4211360</v>
       </c>
       <c r="E226" t="s">
         <v>46</v>
@@ -4572,13 +4585,13 @@
         <v>194</v>
       </c>
       <c r="B227">
-        <v>4282</v>
+        <v>91988</v>
       </c>
       <c r="C227">
         <v>3000</v>
       </c>
       <c r="D227">
-        <v>4211486</v>
+        <v>4662161</v>
       </c>
       <c r="E227" t="s">
         <v>46</v>
@@ -4589,13 +4602,13 @@
         <v>194</v>
       </c>
       <c r="B228">
-        <v>3031</v>
+        <v>4282</v>
       </c>
       <c r="C228">
         <v>3000</v>
       </c>
       <c r="D228">
-        <v>4243797</v>
+        <v>4211486</v>
       </c>
       <c r="E228" t="s">
         <v>46</v>
@@ -4606,13 +4619,13 @@
         <v>194</v>
       </c>
       <c r="B229">
-        <v>3032</v>
+        <v>3031</v>
       </c>
       <c r="C229">
         <v>3000</v>
       </c>
       <c r="D229">
-        <v>4211404</v>
+        <v>4243797</v>
       </c>
       <c r="E229" t="s">
         <v>46</v>
@@ -4623,13 +4636,13 @@
         <v>194</v>
       </c>
       <c r="B230">
-        <v>3035</v>
+        <v>3032</v>
       </c>
       <c r="C230">
         <v>3000</v>
       </c>
       <c r="D230">
-        <v>4211407</v>
+        <v>4211404</v>
       </c>
       <c r="E230" t="s">
         <v>46</v>
@@ -4640,13 +4653,13 @@
         <v>194</v>
       </c>
       <c r="B231">
-        <v>3030</v>
+        <v>3035</v>
       </c>
       <c r="C231">
         <v>3000</v>
       </c>
       <c r="D231">
-        <v>4211402</v>
+        <v>4211407</v>
       </c>
       <c r="E231" t="s">
         <v>46</v>
@@ -4657,13 +4670,13 @@
         <v>194</v>
       </c>
       <c r="B232">
-        <v>3029</v>
+        <v>3030</v>
       </c>
       <c r="C232">
         <v>3000</v>
       </c>
       <c r="D232">
-        <v>4211401</v>
+        <v>4211402</v>
       </c>
       <c r="E232" t="s">
         <v>46</v>
@@ -4674,13 +4687,13 @@
         <v>194</v>
       </c>
       <c r="B233">
-        <v>3958</v>
+        <v>3029</v>
       </c>
       <c r="C233">
         <v>3000</v>
       </c>
       <c r="D233">
-        <v>4211474</v>
+        <v>4211401</v>
       </c>
       <c r="E233" t="s">
         <v>46</v>
@@ -4691,13 +4704,13 @@
         <v>194</v>
       </c>
       <c r="B234">
-        <v>3036</v>
+        <v>3958</v>
       </c>
       <c r="C234">
         <v>3000</v>
       </c>
       <c r="D234">
-        <v>4211408</v>
+        <v>4211474</v>
       </c>
       <c r="E234" t="s">
         <v>46</v>
@@ -4708,13 +4721,13 @@
         <v>194</v>
       </c>
       <c r="B235">
-        <v>3033</v>
+        <v>3036</v>
       </c>
       <c r="C235">
         <v>3000</v>
       </c>
       <c r="D235">
-        <v>4211405</v>
+        <v>4211408</v>
       </c>
       <c r="E235" t="s">
         <v>46</v>
@@ -4725,13 +4738,13 @@
         <v>194</v>
       </c>
       <c r="B236">
-        <v>3028</v>
+        <v>3033</v>
       </c>
       <c r="C236">
         <v>3000</v>
       </c>
       <c r="D236">
-        <v>4211400</v>
+        <v>4211405</v>
       </c>
       <c r="E236" t="s">
         <v>46</v>
@@ -4742,13 +4755,13 @@
         <v>194</v>
       </c>
       <c r="B237">
-        <v>3456</v>
+        <v>3028</v>
       </c>
       <c r="C237">
         <v>3000</v>
       </c>
       <c r="D237">
-        <v>4293831</v>
+        <v>4211400</v>
       </c>
       <c r="E237" t="s">
         <v>46</v>
@@ -4759,13 +4772,13 @@
         <v>194</v>
       </c>
       <c r="B238">
-        <v>3027</v>
+        <v>3456</v>
       </c>
       <c r="C238">
         <v>3000</v>
       </c>
       <c r="D238">
-        <v>4211733</v>
+        <v>4293831</v>
       </c>
       <c r="E238" t="s">
         <v>46</v>
@@ -4776,13 +4789,13 @@
         <v>194</v>
       </c>
       <c r="B239">
-        <v>41539</v>
+        <v>3027</v>
       </c>
       <c r="C239">
         <v>3000</v>
       </c>
       <c r="D239">
-        <v>4166618</v>
+        <v>4211733</v>
       </c>
       <c r="E239" t="s">
         <v>46</v>
@@ -4793,13 +4806,13 @@
         <v>194</v>
       </c>
       <c r="B240">
-        <v>92438</v>
+        <v>41539</v>
       </c>
       <c r="C240">
         <v>3000</v>
       </c>
       <c r="D240">
-        <v>4598522</v>
+        <v>4166618</v>
       </c>
       <c r="E240" t="s">
         <v>46</v>
@@ -4810,13 +4823,13 @@
         <v>194</v>
       </c>
       <c r="B241">
-        <v>91405</v>
+        <v>92438</v>
       </c>
       <c r="C241">
         <v>3000</v>
       </c>
       <c r="D241">
-        <v>4620130</v>
+        <v>4598522</v>
       </c>
       <c r="E241" t="s">
         <v>46</v>
@@ -4824,19 +4837,19 @@
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B242">
-        <v>3024</v>
+        <v>91405</v>
       </c>
       <c r="C242">
         <v>3000</v>
       </c>
       <c r="D242">
-        <v>4210719</v>
+        <v>4620130</v>
       </c>
       <c r="E242" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
@@ -4844,13 +4857,13 @@
         <v>199</v>
       </c>
       <c r="B243">
-        <v>3023</v>
+        <v>3024</v>
       </c>
       <c r="C243">
         <v>3000</v>
       </c>
       <c r="D243">
-        <v>4211063</v>
+        <v>4210719</v>
       </c>
       <c r="E243" t="s">
         <v>47</v>
@@ -4861,13 +4874,13 @@
         <v>199</v>
       </c>
       <c r="B244">
-        <v>3623</v>
+        <v>3023</v>
       </c>
       <c r="C244">
         <v>3000</v>
       </c>
       <c r="D244">
-        <v>4211133</v>
+        <v>4211063</v>
       </c>
       <c r="E244" t="s">
         <v>47</v>
@@ -4878,13 +4891,13 @@
         <v>199</v>
       </c>
       <c r="B245">
-        <v>3710</v>
+        <v>3623</v>
       </c>
       <c r="C245">
         <v>3000</v>
       </c>
       <c r="D245">
-        <v>4211001</v>
+        <v>4211133</v>
       </c>
       <c r="E245" t="s">
         <v>47</v>
@@ -4895,13 +4908,13 @@
         <v>199</v>
       </c>
       <c r="B246">
-        <v>3666</v>
+        <v>3710</v>
       </c>
       <c r="C246">
         <v>3000</v>
       </c>
       <c r="D246">
-        <v>4211056</v>
+        <v>4211001</v>
       </c>
       <c r="E246" t="s">
         <v>47</v>
@@ -4912,13 +4925,13 @@
         <v>199</v>
       </c>
       <c r="B247">
-        <v>3460</v>
+        <v>3666</v>
       </c>
       <c r="C247">
         <v>3000</v>
       </c>
       <c r="D247">
-        <v>4210998</v>
+        <v>4211056</v>
       </c>
       <c r="E247" t="s">
         <v>47</v>
@@ -4929,13 +4942,13 @@
         <v>199</v>
       </c>
       <c r="B248">
-        <v>4477</v>
+        <v>3460</v>
       </c>
       <c r="C248">
         <v>3000</v>
       </c>
       <c r="D248">
-        <v>4257526</v>
+        <v>4210998</v>
       </c>
       <c r="E248" t="s">
         <v>47</v>
@@ -4946,13 +4959,13 @@
         <v>199</v>
       </c>
       <c r="B249">
-        <v>60479</v>
+        <v>4477</v>
       </c>
       <c r="C249">
         <v>3000</v>
       </c>
       <c r="D249">
-        <v>6133611</v>
+        <v>4257526</v>
       </c>
       <c r="E249" t="s">
         <v>47</v>
@@ -4963,13 +4976,13 @@
         <v>199</v>
       </c>
       <c r="B250">
-        <v>3022</v>
+        <v>60479</v>
       </c>
       <c r="C250">
         <v>3000</v>
       </c>
       <c r="D250">
-        <v>4211094</v>
+        <v>6133611</v>
       </c>
       <c r="E250" t="s">
         <v>47</v>
@@ -4980,13 +4993,13 @@
         <v>199</v>
       </c>
       <c r="B251">
-        <v>3021</v>
+        <v>3022</v>
       </c>
       <c r="C251">
         <v>3000</v>
       </c>
       <c r="D251">
-        <v>4211043</v>
+        <v>4211094</v>
       </c>
       <c r="E251" t="s">
         <v>47</v>
@@ -4997,13 +5010,13 @@
         <v>199</v>
       </c>
       <c r="B252">
-        <v>3020</v>
+        <v>3021</v>
       </c>
       <c r="C252">
         <v>3000</v>
       </c>
       <c r="D252">
-        <v>4211065</v>
+        <v>4211043</v>
       </c>
       <c r="E252" t="s">
         <v>47</v>
@@ -5014,13 +5027,13 @@
         <v>199</v>
       </c>
       <c r="B253">
-        <v>3795</v>
+        <v>3020</v>
       </c>
       <c r="C253">
         <v>3000</v>
       </c>
       <c r="D253">
-        <v>4211002</v>
+        <v>4211065</v>
       </c>
       <c r="E253" t="s">
         <v>47</v>
@@ -5031,13 +5044,13 @@
         <v>199</v>
       </c>
       <c r="B254">
-        <v>3034</v>
+        <v>3795</v>
       </c>
       <c r="C254">
         <v>3000</v>
       </c>
       <c r="D254">
-        <v>4210997</v>
+        <v>4211002</v>
       </c>
       <c r="E254" t="s">
         <v>47</v>
@@ -5048,13 +5061,13 @@
         <v>199</v>
       </c>
       <c r="B255">
-        <v>3832</v>
+        <v>3034</v>
       </c>
       <c r="C255">
         <v>3000</v>
       </c>
       <c r="D255">
-        <v>4210678</v>
+        <v>4210997</v>
       </c>
       <c r="E255" t="s">
         <v>47</v>
@@ -5065,13 +5078,13 @@
         <v>199</v>
       </c>
       <c r="B256">
-        <v>2445</v>
+        <v>3832</v>
       </c>
       <c r="C256">
         <v>3000</v>
       </c>
       <c r="D256">
-        <v>4211067</v>
+        <v>4210678</v>
       </c>
       <c r="E256" t="s">
         <v>47</v>
@@ -5082,13 +5095,13 @@
         <v>199</v>
       </c>
       <c r="B257">
-        <v>91988</v>
+        <v>2445</v>
       </c>
       <c r="C257">
         <v>3000</v>
       </c>
       <c r="D257">
-        <v>6000970</v>
+        <v>4211067</v>
       </c>
       <c r="E257" t="s">
         <v>47</v>
@@ -5099,13 +5112,13 @@
         <v>199</v>
       </c>
       <c r="B258">
-        <v>4282</v>
+        <v>91988</v>
       </c>
       <c r="C258">
         <v>3000</v>
       </c>
       <c r="D258">
-        <v>4210796</v>
+        <v>6000970</v>
       </c>
       <c r="E258" t="s">
         <v>47</v>
@@ -5116,13 +5129,13 @@
         <v>199</v>
       </c>
       <c r="B259">
-        <v>3031</v>
+        <v>4282</v>
       </c>
       <c r="C259">
         <v>3000</v>
       </c>
       <c r="D259">
-        <v>4243831</v>
+        <v>4210796</v>
       </c>
       <c r="E259" t="s">
         <v>47</v>
@@ -5133,13 +5146,13 @@
         <v>199</v>
       </c>
       <c r="B260">
-        <v>3032</v>
+        <v>3031</v>
       </c>
       <c r="C260">
         <v>3000</v>
       </c>
       <c r="D260">
-        <v>4211115</v>
+        <v>4243831</v>
       </c>
       <c r="E260" t="s">
         <v>47</v>
@@ -5150,13 +5163,13 @@
         <v>199</v>
       </c>
       <c r="B261">
-        <v>3035</v>
+        <v>3032</v>
       </c>
       <c r="C261">
         <v>3000</v>
       </c>
       <c r="D261">
-        <v>4211061</v>
+        <v>4211115</v>
       </c>
       <c r="E261" t="s">
         <v>47</v>
@@ -5167,13 +5180,13 @@
         <v>199</v>
       </c>
       <c r="B262">
-        <v>3030</v>
+        <v>3035</v>
       </c>
       <c r="C262">
         <v>3000</v>
       </c>
       <c r="D262">
-        <v>4211122</v>
+        <v>4211061</v>
       </c>
       <c r="E262" t="s">
         <v>47</v>
@@ -5184,13 +5197,13 @@
         <v>199</v>
       </c>
       <c r="B263">
-        <v>3029</v>
+        <v>3030</v>
       </c>
       <c r="C263">
         <v>3000</v>
       </c>
       <c r="D263">
-        <v>4210706</v>
+        <v>4211122</v>
       </c>
       <c r="E263" t="s">
         <v>47</v>
@@ -5201,13 +5214,13 @@
         <v>199</v>
       </c>
       <c r="B264">
-        <v>3958</v>
+        <v>3029</v>
       </c>
       <c r="C264">
         <v>3000</v>
       </c>
       <c r="D264">
-        <v>4211134</v>
+        <v>4210706</v>
       </c>
       <c r="E264" t="s">
         <v>47</v>
@@ -5218,13 +5231,13 @@
         <v>199</v>
       </c>
       <c r="B265">
-        <v>3036</v>
+        <v>3958</v>
       </c>
       <c r="C265">
         <v>3000</v>
       </c>
       <c r="D265">
-        <v>4210794</v>
+        <v>4211134</v>
       </c>
       <c r="E265" t="s">
         <v>47</v>
@@ -5235,13 +5248,13 @@
         <v>199</v>
       </c>
       <c r="B266">
-        <v>3033</v>
+        <v>3036</v>
       </c>
       <c r="C266">
         <v>3000</v>
       </c>
       <c r="D266">
-        <v>4211114</v>
+        <v>4210794</v>
       </c>
       <c r="E266" t="s">
         <v>47</v>
@@ -5252,13 +5265,13 @@
         <v>199</v>
       </c>
       <c r="B267">
-        <v>3028</v>
+        <v>3033</v>
       </c>
       <c r="C267">
         <v>3000</v>
       </c>
       <c r="D267">
-        <v>4256149</v>
+        <v>4211114</v>
       </c>
       <c r="E267" t="s">
         <v>47</v>
@@ -5269,13 +5282,13 @@
         <v>199</v>
       </c>
       <c r="B268">
-        <v>3456</v>
+        <v>3028</v>
       </c>
       <c r="C268">
         <v>3000</v>
       </c>
       <c r="D268">
-        <v>4210720</v>
+        <v>4256149</v>
       </c>
       <c r="E268" t="s">
         <v>47</v>
@@ -5286,13 +5299,13 @@
         <v>199</v>
       </c>
       <c r="B269">
-        <v>3027</v>
+        <v>3456</v>
       </c>
       <c r="C269">
         <v>3000</v>
       </c>
       <c r="D269">
-        <v>4226358</v>
+        <v>4210720</v>
       </c>
       <c r="E269" t="s">
         <v>47</v>
@@ -5303,13 +5316,13 @@
         <v>199</v>
       </c>
       <c r="B270">
-        <v>41539</v>
+        <v>3027</v>
       </c>
       <c r="C270">
         <v>3000</v>
       </c>
       <c r="D270">
-        <v>4210802</v>
+        <v>4226358</v>
       </c>
       <c r="E270" t="s">
         <v>47</v>
@@ -5320,13 +5333,13 @@
         <v>199</v>
       </c>
       <c r="B271">
-        <v>92438</v>
+        <v>41539</v>
       </c>
       <c r="C271">
         <v>3000</v>
       </c>
       <c r="D271">
-        <v>4654613</v>
+        <v>4210802</v>
       </c>
       <c r="E271" t="s">
         <v>47</v>
@@ -5337,13 +5350,13 @@
         <v>199</v>
       </c>
       <c r="B272">
-        <v>91405</v>
+        <v>92438</v>
       </c>
       <c r="C272">
         <v>3000</v>
       </c>
       <c r="D272">
-        <v>6004927</v>
+        <v>4654613</v>
       </c>
       <c r="E272" t="s">
         <v>47</v>
@@ -5351,19 +5364,19 @@
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273">
-        <v>330</v>
+        <v>199</v>
       </c>
       <c r="B273">
-        <v>3024</v>
+        <v>91405</v>
       </c>
       <c r="C273">
         <v>3000</v>
       </c>
       <c r="D273">
-        <v>6058245</v>
+        <v>6004927</v>
       </c>
       <c r="E273" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
@@ -5371,13 +5384,13 @@
         <v>330</v>
       </c>
       <c r="B274">
-        <v>3023</v>
+        <v>3024</v>
       </c>
       <c r="C274">
         <v>3000</v>
       </c>
       <c r="D274">
-        <v>6016483</v>
+        <v>6058245</v>
       </c>
       <c r="E274" t="s">
         <v>50</v>
@@ -5388,13 +5401,13 @@
         <v>330</v>
       </c>
       <c r="B275">
-        <v>3623</v>
+        <v>3023</v>
       </c>
       <c r="C275">
         <v>3000</v>
       </c>
       <c r="D275">
-        <v>6278088</v>
+        <v>6016483</v>
       </c>
       <c r="E275" t="s">
         <v>50</v>
@@ -5405,13 +5418,13 @@
         <v>330</v>
       </c>
       <c r="B276">
-        <v>3460</v>
+        <v>3623</v>
       </c>
       <c r="C276">
         <v>3000</v>
       </c>
       <c r="D276">
-        <v>6278034</v>
+        <v>6278088</v>
       </c>
       <c r="E276" t="s">
         <v>50</v>
@@ -5422,13 +5435,13 @@
         <v>330</v>
       </c>
       <c r="B277">
-        <v>3022</v>
+        <v>3460</v>
       </c>
       <c r="C277">
         <v>3000</v>
       </c>
       <c r="D277">
-        <v>6079617</v>
+        <v>6278034</v>
       </c>
       <c r="E277" t="s">
         <v>50</v>
@@ -5439,13 +5452,13 @@
         <v>330</v>
       </c>
       <c r="B278">
-        <v>3020</v>
+        <v>3022</v>
       </c>
       <c r="C278">
-        <v>0</v>
-      </c>
-      <c r="D278" s="1">
-        <v>6020144</v>
+        <v>3000</v>
+      </c>
+      <c r="D278">
+        <v>6079617</v>
       </c>
       <c r="E278" t="s">
         <v>50</v>
@@ -5456,13 +5469,13 @@
         <v>330</v>
       </c>
       <c r="B279">
-        <v>3034</v>
+        <v>3020</v>
       </c>
       <c r="C279">
-        <v>3000</v>
-      </c>
-      <c r="D279">
-        <v>6273296</v>
+        <v>0</v>
+      </c>
+      <c r="D279" s="1">
+        <v>6020144</v>
       </c>
       <c r="E279" t="s">
         <v>50</v>
@@ -5473,13 +5486,13 @@
         <v>330</v>
       </c>
       <c r="B280">
-        <v>92438</v>
+        <v>3034</v>
       </c>
       <c r="C280">
         <v>3000</v>
       </c>
       <c r="D280">
-        <v>6272108</v>
+        <v>6273296</v>
       </c>
       <c r="E280" t="s">
         <v>50</v>
@@ -5487,19 +5500,19 @@
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281">
-        <v>37</v>
+        <v>330</v>
       </c>
       <c r="B281">
-        <v>3070</v>
+        <v>92438</v>
       </c>
       <c r="C281">
         <v>3000</v>
       </c>
       <c r="D281">
-        <v>6172375</v>
+        <v>6272108</v>
       </c>
       <c r="E281" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
@@ -5507,13 +5520,13 @@
         <v>37</v>
       </c>
       <c r="B282">
-        <v>3069</v>
+        <v>3070</v>
       </c>
       <c r="C282">
         <v>3000</v>
       </c>
       <c r="D282">
-        <v>6195258</v>
+        <v>6172375</v>
       </c>
       <c r="E282" t="s">
         <v>44</v>
@@ -5524,13 +5537,13 @@
         <v>37</v>
       </c>
       <c r="B283">
-        <v>2431</v>
+        <v>3069</v>
       </c>
       <c r="C283">
         <v>3000</v>
       </c>
       <c r="D283">
-        <v>6195267</v>
+        <v>6195258</v>
       </c>
       <c r="E283" t="s">
         <v>44</v>
@@ -5541,13 +5554,13 @@
         <v>37</v>
       </c>
       <c r="B284">
-        <v>3068</v>
+        <v>2431</v>
       </c>
       <c r="C284">
         <v>3000</v>
       </c>
       <c r="D284">
-        <v>6294513</v>
+        <v>6195267</v>
       </c>
       <c r="E284" t="s">
         <v>44</v>
@@ -5558,13 +5571,13 @@
         <v>37</v>
       </c>
       <c r="B285">
-        <v>87079</v>
+        <v>3068</v>
       </c>
       <c r="C285">
         <v>3000</v>
       </c>
       <c r="D285">
-        <v>6173814</v>
+        <v>6294513</v>
       </c>
       <c r="E285" t="s">
         <v>44</v>
@@ -5572,19 +5585,19 @@
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286">
-        <v>140</v>
+        <v>37</v>
       </c>
       <c r="B286">
-        <v>3070</v>
+        <v>87079</v>
       </c>
       <c r="C286">
         <v>3000</v>
       </c>
       <c r="D286">
-        <v>4631385</v>
+        <v>6173814</v>
       </c>
       <c r="E286" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
@@ -5592,13 +5605,13 @@
         <v>140</v>
       </c>
       <c r="B287">
-        <v>3069</v>
+        <v>3070</v>
       </c>
       <c r="C287">
         <v>3000</v>
       </c>
       <c r="D287">
-        <v>4528488</v>
+        <v>4631385</v>
       </c>
       <c r="E287" t="s">
         <v>53</v>
@@ -5609,13 +5622,13 @@
         <v>140</v>
       </c>
       <c r="B288">
-        <v>63864</v>
+        <v>3069</v>
       </c>
       <c r="C288">
         <v>3000</v>
       </c>
       <c r="D288">
-        <v>6132566</v>
+        <v>4528488</v>
       </c>
       <c r="E288" t="s">
         <v>53</v>
@@ -5626,13 +5639,13 @@
         <v>140</v>
       </c>
       <c r="B289">
-        <v>2431</v>
+        <v>63864</v>
       </c>
       <c r="C289">
         <v>3000</v>
       </c>
       <c r="D289">
-        <v>6103985</v>
+        <v>6132566</v>
       </c>
       <c r="E289" t="s">
         <v>53</v>
@@ -5643,13 +5656,13 @@
         <v>140</v>
       </c>
       <c r="B290">
-        <v>6636</v>
+        <v>2431</v>
       </c>
       <c r="C290">
         <v>3000</v>
       </c>
       <c r="D290">
-        <v>4252437</v>
+        <v>6103985</v>
       </c>
       <c r="E290" t="s">
         <v>53</v>
@@ -5660,13 +5673,13 @@
         <v>140</v>
       </c>
       <c r="B291">
-        <v>3068</v>
+        <v>6636</v>
       </c>
       <c r="C291">
         <v>3000</v>
       </c>
       <c r="D291">
-        <v>4205004</v>
+        <v>4252437</v>
       </c>
       <c r="E291" t="s">
         <v>53</v>
@@ -5677,13 +5690,13 @@
         <v>140</v>
       </c>
       <c r="B292">
-        <v>26603</v>
+        <v>3068</v>
       </c>
       <c r="C292">
         <v>3000</v>
       </c>
       <c r="D292">
-        <v>6186974</v>
+        <v>4205004</v>
       </c>
       <c r="E292" t="s">
         <v>53</v>
@@ -5694,13 +5707,13 @@
         <v>140</v>
       </c>
       <c r="B293">
-        <v>87079</v>
+        <v>26603</v>
       </c>
       <c r="C293">
         <v>3000</v>
       </c>
       <c r="D293">
-        <v>4569836</v>
+        <v>6186974</v>
       </c>
       <c r="E293" t="s">
         <v>53</v>
@@ -5708,19 +5721,19 @@
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294">
-        <v>321</v>
+        <v>140</v>
       </c>
       <c r="B294">
-        <v>3070</v>
+        <v>87079</v>
       </c>
       <c r="C294">
         <v>3000</v>
       </c>
       <c r="D294">
-        <v>6151658</v>
+        <v>4569836</v>
       </c>
       <c r="E294" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
@@ -5728,13 +5741,13 @@
         <v>321</v>
       </c>
       <c r="B295">
-        <v>3069</v>
+        <v>3070</v>
       </c>
       <c r="C295">
         <v>3000</v>
       </c>
       <c r="D295">
-        <v>6151659</v>
+        <v>6151658</v>
       </c>
       <c r="E295" t="s">
         <v>77</v>
@@ -5745,13 +5758,13 @@
         <v>321</v>
       </c>
       <c r="B296">
-        <v>2431</v>
+        <v>3069</v>
       </c>
       <c r="C296">
         <v>3000</v>
       </c>
       <c r="D296">
-        <v>6205089</v>
+        <v>6151659</v>
       </c>
       <c r="E296" t="s">
         <v>77</v>
@@ -5762,13 +5775,13 @@
         <v>321</v>
       </c>
       <c r="B297">
-        <v>6636</v>
+        <v>2431</v>
       </c>
       <c r="C297">
         <v>3000</v>
       </c>
       <c r="D297">
-        <v>6164336</v>
+        <v>6205089</v>
       </c>
       <c r="E297" t="s">
         <v>77</v>
@@ -5779,13 +5792,13 @@
         <v>321</v>
       </c>
       <c r="B298">
-        <v>3068</v>
+        <v>6636</v>
       </c>
       <c r="C298">
         <v>3000</v>
       </c>
       <c r="D298">
-        <v>6205087</v>
+        <v>6164336</v>
       </c>
       <c r="E298" t="s">
         <v>77</v>
@@ -5796,13 +5809,13 @@
         <v>321</v>
       </c>
       <c r="B299">
-        <v>87079</v>
+        <v>3068</v>
       </c>
       <c r="C299">
         <v>3000</v>
       </c>
       <c r="D299">
-        <v>6206312</v>
+        <v>6205087</v>
       </c>
       <c r="E299" t="s">
         <v>77</v>
@@ -5810,19 +5823,19 @@
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300">
-        <v>37</v>
+        <v>321</v>
       </c>
       <c r="B300">
-        <v>3004</v>
+        <v>87079</v>
       </c>
       <c r="C300">
         <v>3000</v>
       </c>
       <c r="D300">
-        <v>4647553</v>
+        <v>6206312</v>
       </c>
       <c r="E300" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
@@ -5830,13 +5843,13 @@
         <v>37</v>
       </c>
       <c r="B301">
-        <v>3003</v>
+        <v>3004</v>
       </c>
       <c r="C301">
-        <v>0</v>
-      </c>
-      <c r="D301" s="1">
-        <v>4209117</v>
+        <v>3000</v>
+      </c>
+      <c r="D301">
+        <v>4647553</v>
       </c>
       <c r="E301" t="s">
         <v>44</v>
@@ -5844,19 +5857,19 @@
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302">
-        <v>140</v>
+        <v>37</v>
       </c>
       <c r="B302">
-        <v>3005</v>
+        <v>3003</v>
       </c>
       <c r="C302">
-        <v>3000</v>
-      </c>
-      <c r="D302">
-        <v>4255413</v>
+        <v>0</v>
+      </c>
+      <c r="D302" s="1">
+        <v>4209117</v>
       </c>
       <c r="E302" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
@@ -5864,13 +5877,13 @@
         <v>140</v>
       </c>
       <c r="B303">
-        <v>3004</v>
+        <v>3005</v>
       </c>
       <c r="C303">
         <v>3000</v>
       </c>
       <c r="D303">
-        <v>4249891</v>
+        <v>4255413</v>
       </c>
       <c r="E303" t="s">
         <v>53</v>
@@ -5881,13 +5894,13 @@
         <v>140</v>
       </c>
       <c r="B304">
-        <v>3622</v>
+        <v>3004</v>
       </c>
       <c r="C304">
         <v>3000</v>
       </c>
       <c r="D304">
-        <v>6233955</v>
+        <v>4249891</v>
       </c>
       <c r="E304" t="s">
         <v>53</v>
@@ -5898,13 +5911,13 @@
         <v>140</v>
       </c>
       <c r="B305">
-        <v>3010</v>
+        <v>3622</v>
       </c>
       <c r="C305">
         <v>3000</v>
       </c>
       <c r="D305">
-        <v>4264569</v>
+        <v>6233955</v>
       </c>
       <c r="E305" t="s">
         <v>53</v>
@@ -5915,13 +5928,13 @@
         <v>140</v>
       </c>
       <c r="B306">
-        <v>3009</v>
+        <v>3010</v>
       </c>
       <c r="C306">
         <v>3000</v>
       </c>
       <c r="D306">
-        <v>6221672</v>
+        <v>4264569</v>
       </c>
       <c r="E306" t="s">
         <v>53</v>
@@ -5932,13 +5945,13 @@
         <v>140</v>
       </c>
       <c r="B307">
-        <v>3008</v>
+        <v>3009</v>
       </c>
       <c r="C307">
         <v>3000</v>
       </c>
       <c r="D307">
-        <v>6277303</v>
+        <v>6221672</v>
       </c>
       <c r="E307" t="s">
         <v>53</v>
@@ -5949,13 +5962,13 @@
         <v>140</v>
       </c>
       <c r="B308">
-        <v>6111</v>
+        <v>3008</v>
       </c>
       <c r="C308">
         <v>3000</v>
       </c>
       <c r="D308">
-        <v>6224700</v>
+        <v>6277303</v>
       </c>
       <c r="E308" t="s">
         <v>53</v>
@@ -5966,13 +5979,13 @@
         <v>140</v>
       </c>
       <c r="B309">
-        <v>2465</v>
+        <v>6111</v>
       </c>
       <c r="C309">
         <v>3000</v>
       </c>
       <c r="D309">
-        <v>6258407</v>
+        <v>6224700</v>
       </c>
       <c r="E309" t="s">
         <v>53</v>
@@ -5983,13 +5996,13 @@
         <v>140</v>
       </c>
       <c r="B310">
-        <v>3003</v>
+        <v>2465</v>
       </c>
       <c r="C310">
         <v>3000</v>
       </c>
       <c r="D310">
-        <v>4296785</v>
+        <v>6258407</v>
       </c>
       <c r="E310" t="s">
         <v>53</v>
@@ -6000,13 +6013,13 @@
         <v>140</v>
       </c>
       <c r="B311">
-        <v>3001</v>
+        <v>3003</v>
       </c>
       <c r="C311">
-        <v>0</v>
-      </c>
-      <c r="D311" s="1">
-        <v>4530029</v>
+        <v>3000</v>
+      </c>
+      <c r="D311">
+        <v>4296785</v>
       </c>
       <c r="E311" t="s">
         <v>53</v>
@@ -6017,22 +6030,42 @@
         <v>140</v>
       </c>
       <c r="B312">
-        <v>3007</v>
+        <v>3001</v>
       </c>
       <c r="C312">
         <v>0</v>
       </c>
       <c r="D312" s="1">
-        <v>4275782</v>
+        <v>4530029</v>
       </c>
       <c r="E312" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="313" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G313" s="1"/>
+      <c r="A313">
+        <v>140</v>
+      </c>
+      <c r="B313">
+        <v>3007</v>
+      </c>
+      <c r="C313">
+        <v>0</v>
+      </c>
+      <c r="D313" s="1">
+        <v>4275782</v>
+      </c>
+      <c r="E313" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G314" s="1"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A59:E83">
+    <sortCondition ref="B59:B83"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6041,9 +6074,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7AA3FC-C182-4F86-A259-25CEBC625BE2}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33:A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>